<commit_message>
updates restassure contact us
</commit_message>
<xml_diff>
--- a/Ecommerse_RestAssured_shilpa/src/test/resources/project_documents.xlsx
+++ b/Ecommerse_RestAssured_shilpa/src/test/resources/project_documents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationScriptsFiles\project_management_tool_jira\ecommese_parallel_testing_shilpa\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationScriptsFiles\project_management_tool_jira\Ecommerse_RestAssured_shilpa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92364D6A-1E1F-4BD4-9A0E-1C81FB573A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5843B5-A882-4CF7-83B8-EDA924BB96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Loginpage" sheetId="4" r:id="rId4"/>
     <sheet name="Wishlistpage" sheetId="5" r:id="rId5"/>
     <sheet name="searchproductpage" sheetId="6" r:id="rId6"/>
+    <sheet name="contact" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="313">
   <si>
     <t>header elements</t>
   </si>
@@ -952,6 +953,18 @@
   </si>
   <si>
     <t>Search-Products | ECODERS</t>
+  </si>
+  <si>
+    <t>shilpaNMurthy</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>shilpa@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hi hello </t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1043,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1040,6 +1053,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2770,7 +2784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E52AA66-FDE9-4DA7-8BAC-2C518FABDDD3}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2784,4 +2798,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1832889-0A2B-4757-B03E-71D0CD2307D1}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1">
+        <v>1234567892</v>
+      </c>
+      <c r="E1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{CE110A46-047D-48D8-81F9-18370175DB07}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>